<commit_message>
Test Suite - API - 12/05/2022
</commit_message>
<xml_diff>
--- a/data-test/WEB_Login.xlsx
+++ b/data-test/WEB_Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta\data-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B67F133-6F6F-4025-B623-26F0BE574A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB94956-67C5-47E1-964E-FCD9A59CA133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="3120" windowWidth="18000" windowHeight="9270" xr2:uid="{8F5F9D6E-79FD-43CA-8996-71E85E16DC5F}"/>
+    <workbookView xWindow="4950" yWindow="3315" windowWidth="18000" windowHeight="9270" xr2:uid="{8F5F9D6E-79FD-43CA-8996-71E85E16DC5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,12 +125,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,7 +450,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,67 +461,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test Suite Web - 14/05/2022
</commit_message>
<xml_diff>
--- a/data-test/WEB_Login.xlsx
+++ b/data-test/WEB_Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\final-project-qe-alta4\final-project-qe-alta\data-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB94956-67C5-47E1-964E-FCD9A59CA133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050665FE-A01E-4403-BD3C-265F76ED7E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="3315" windowWidth="18000" windowHeight="9270" xr2:uid="{8F5F9D6E-79FD-43CA-8996-71E85E16DC5F}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9270" xr2:uid="{8F5F9D6E-79FD-43CA-8996-71E85E16DC5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>positive</t>
+  </si>
+  <si>
+    <t>halosalsa</t>
   </si>
 </sst>
 </file>
@@ -125,13 +128,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -447,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCA34FA-69A3-4016-BDF7-A057E44DD216}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,20 +530,36 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{F1D49744-BAD1-453E-874F-004E57C56B8B}"/>
     <hyperlink ref="A6" r:id="rId2" xr:uid="{ECCAA25F-1E47-4DC4-AF46-ABB61EF4A619}"/>
-    <hyperlink ref="A7" r:id="rId3" xr:uid="{F849857C-3068-468B-8F57-CA7617E7C82B}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{F849857C-3068-468B-8F57-CA7617E7C82B}"/>
     <hyperlink ref="A4" r:id="rId4" xr:uid="{A3C7F5E1-A92C-4987-AEA2-7E4D975B0ED1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>